<commit_message>
Data Driven Testing added for User Sign Up Page....
</commit_message>
<xml_diff>
--- a/onLineShoppingProject/src/main/java/com/e_commerce/qa/testdata/SignUpUser.xlsx
+++ b/onLineShoppingProject/src/main/java/com/e_commerce/qa/testdata/SignUpUser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Drivers\ExcelUtilsFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA3CC08-49F3-4C27-91DA-9D0147A51D24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A45BC22-E09B-4697-B151-8AB27FB7C15A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3630" yWindow="1830" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>First Name</t>
   </si>
@@ -48,27 +48,12 @@
     <t>City</t>
   </si>
   <si>
-    <t>Postal Code</t>
-  </si>
-  <si>
-    <t>Mobile No.</t>
-  </si>
-  <si>
     <t>Alias</t>
   </si>
   <si>
     <t>Email_Id</t>
   </si>
   <si>
-    <t>opq@gmail.com</t>
-  </si>
-  <si>
-    <t>nop@yahoomail.com</t>
-  </si>
-  <si>
-    <t>miss@gmail.com</t>
-  </si>
-  <si>
     <t>Tom</t>
   </si>
   <si>
@@ -121,6 +106,39 @@
   </si>
   <si>
     <t>Cooper</t>
+  </si>
+  <si>
+    <t>Zip code</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>98765</t>
+  </si>
+  <si>
+    <t>54321</t>
+  </si>
+  <si>
+    <t>6472152005</t>
+  </si>
+  <si>
+    <t>6472152003</t>
+  </si>
+  <si>
+    <t>6472152002</t>
+  </si>
+  <si>
+    <t>tester123@yahoomail.com</t>
+  </si>
+  <si>
+    <t>tester1234@gmail.com</t>
+  </si>
+  <si>
+    <t>tester987@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -192,10 +210,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -482,7 +500,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +510,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -516,118 +534,118 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="4">
-        <v>12345</v>
-      </c>
-      <c r="J2" s="4">
-        <v>6472152005</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>29</v>
+      <c r="G2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="4">
-        <v>98765</v>
-      </c>
-      <c r="J3" s="4">
-        <v>6472152004</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>31</v>
+      <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="4">
-        <v>21055</v>
-      </c>
-      <c r="J4" s="4">
-        <v>6472152003</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>